<commit_message>
Grupo C taller 1 calificado
</commit_message>
<xml_diff>
--- a/MONITOR20-2/GC/Taller1/revisiónTaller1.xlsx
+++ b/MONITOR20-2/GC/Taller1/revisiónTaller1.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BDB497-B979-47E2-A1A8-69341E13D233}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A8EB17B-94FC-46D8-BC1E-31D6DCEA3860}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>NO.</t>
   </si>
@@ -135,6 +135,21 @@
   </si>
   <si>
     <t>Vera Campo,Valentina</t>
+  </si>
+  <si>
+    <t>(El punto 6 parece copiado de internet)</t>
+  </si>
+  <si>
+    <t>(En algunas partes usa conceptos no vistos y entregó los archivos en .txt pero todo se ve bien)</t>
+  </si>
+  <si>
+    <t>(En el punto 6 los números no están invertidos, solo imprimió los dígitos)</t>
+  </si>
+  <si>
+    <t>(En el punto 6 los números no están invertidos, solo imprimió los dígitos)(En el punto 5 le falta parentesís (2*a), el programa no da un resultado correcto)</t>
+  </si>
+  <si>
+    <t>En el punto 5 le falta parentesís (2*a), el programa no da un resultado correcto</t>
   </si>
 </sst>
 </file>
@@ -281,7 +296,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -312,6 +327,10 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,7 +349,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -629,21 +648,22 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
     <col min="2" max="2" width="0.140625" customWidth="1"/>
     <col min="3" max="3" width="33.7109375" customWidth="1"/>
     <col min="4" max="10" width="5.5703125" customWidth="1"/>
+    <col min="11" max="11" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="15.75" customHeight="1" thickBot="1">
+    <row r="1" spans="1:11" ht="15.75" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>9</v>
       </c>
@@ -657,7 +677,7 @@
       <c r="I1" s="8"/>
       <c r="J1" s="8"/>
     </row>
-    <row r="2" spans="1:10" ht="39" customHeight="1" thickBot="1">
+    <row r="2" spans="1:11" ht="39" customHeight="1" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,7 +707,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:11">
       <c r="A3" s="4">
         <v>1</v>
       </c>
@@ -695,8 +715,29 @@
       <c r="C3" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:10">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="4">
         <v>2</v>
       </c>
@@ -704,8 +745,29 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:10">
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="4">
         <v>3</v>
       </c>
@@ -713,8 +775,32 @@
       <c r="C5" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>2</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="4">
         <v>4</v>
       </c>
@@ -722,8 +808,32 @@
       <c r="C6" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="4">
         <v>5</v>
       </c>
@@ -731,8 +841,32 @@
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="8" spans="1:10">
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+      <c r="I7">
+        <v>2</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -740,8 +874,29 @@
       <c r="C8" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="9" spans="1:10">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>1</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>1</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -749,8 +904,29 @@
       <c r="C9" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="10" spans="1:10">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>1</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -758,8 +934,29 @@
       <c r="C10" s="6" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="11" spans="1:10">
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>1</v>
+      </c>
+      <c r="I10">
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -767,8 +964,29 @@
       <c r="C11" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" spans="1:10">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11">
+        <v>1</v>
+      </c>
+      <c r="I11">
+        <v>1</v>
+      </c>
+      <c r="J11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -776,8 +994,29 @@
       <c r="C12" s="6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="13" spans="1:10">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>1</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -785,8 +1024,29 @@
       <c r="C13" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="14" spans="1:10">
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -794,8 +1054,32 @@
       <c r="C14" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:10">
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14">
+        <v>1</v>
+      </c>
+      <c r="I14">
+        <v>2</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -803,8 +1087,29 @@
       <c r="C15" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>1</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -812,8 +1117,29 @@
       <c r="C16" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:3">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>1</v>
+      </c>
+      <c r="J16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -821,8 +1147,29 @@
       <c r="C17" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:3">
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -830,8 +1177,32 @@
       <c r="C18" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:3">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1</v>
+      </c>
+      <c r="F18">
+        <v>1</v>
+      </c>
+      <c r="G18">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>2</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -839,8 +1210,29 @@
       <c r="C19" s="6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="20" spans="1:3">
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>1</v>
+      </c>
+      <c r="G19">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+      <c r="I19">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -848,8 +1240,32 @@
       <c r="C20" s="6" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="21" spans="1:3">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>1</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -857,8 +1273,29 @@
       <c r="C21" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="22" spans="1:3">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>1</v>
+      </c>
+      <c r="F21">
+        <v>1</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>1</v>
+      </c>
+      <c r="J21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -866,8 +1303,29 @@
       <c r="C22" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:3">
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>1</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>1</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -875,8 +1333,32 @@
       <c r="C23" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="24" spans="1:3">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>1</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>2</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -884,8 +1366,29 @@
       <c r="C24" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="25" spans="1:3">
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>1</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -893,8 +1396,29 @@
       <c r="C25" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="1:3">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>1</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+      <c r="I25">
+        <v>1</v>
+      </c>
+      <c r="J25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -902,8 +1426,29 @@
       <c r="C26" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="1:3">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>1</v>
+      </c>
+      <c r="I26">
+        <v>1</v>
+      </c>
+      <c r="J26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -911,8 +1456,29 @@
       <c r="C27" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="28" spans="1:3">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>1</v>
+      </c>
+      <c r="F27">
+        <v>1</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>1</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -920,8 +1486,29 @@
       <c r="C28" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>1</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>0</v>
+      </c>
+      <c r="I28">
+        <v>1</v>
+      </c>
+      <c r="J28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="37.5" customHeight="1">
       <c r="A29" s="4">
         <v>27</v>
       </c>
@@ -929,8 +1516,37 @@
       <c r="C29" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="30" spans="1:3">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+      <c r="F29">
+        <v>1</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>2</v>
+      </c>
+      <c r="I29">
+        <v>2</v>
+      </c>
+      <c r="J29">
+        <v>1</v>
+      </c>
+      <c r="K29" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="10"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="4">
         <v>28</v>
       </c>
@@ -938,8 +1554,32 @@
       <c r="C30" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="1:3">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>1</v>
+      </c>
+      <c r="F30">
+        <v>1</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>2</v>
+      </c>
+      <c r="J30">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="4">
         <v>29</v>
       </c>
@@ -947,10 +1587,35 @@
       <c r="C31" s="6" t="s">
         <v>38</v>
       </c>
+      <c r="D31">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>1</v>
+      </c>
+      <c r="F31">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>2</v>
+      </c>
+      <c r="J31">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:J1"/>
+    <mergeCell ref="K29:O29"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup orientation="landscape" r:id="rId1"/>

</xml_diff>